<commit_message>
Chapter20 Automatic Form Filler, 5 forms, data from excel file
</commit_message>
<xml_diff>
--- a/Chapter 20 – Controlling the Keyboard and Mouse with GUI Automation/automatic_form_fller/data_for_the_form.xlsx
+++ b/Chapter 20 – Controlling the Keyboard and Mouse with GUI Automation/automatic_form_fller/data_for_the_form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\Automate the Boring Stuff with Python\Chapter 20 – Controlling the Keyboard and Mouse with GUI Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\Automate the Boring Stuff with Python\Chapter 20 – Controlling the Keyboard and Mouse with GUI Automation\automatic_form_fller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D0DC7D-607E-4537-823C-6AD78E9F62B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E2DCF-8D03-4B00-883A-FC37A107F889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11325" xr2:uid="{F9B3A74F-49E0-441D-9CCD-002DCF291DD1}"/>
+    <workbookView xWindow="0" yWindow="552" windowWidth="21600" windowHeight="11328" xr2:uid="{F9B3A74F-49E0-441D-9CCD-002DCF291DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Robocop</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John </t>
+  </si>
+  <si>
+    <t>Dirty dishes</t>
+  </si>
+  <si>
+    <t>Have a nice day</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3391B21-C4C9-451A-9760-EAF41DA4112D}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,6 +565,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>